<commit_message>
Working on finishing CalcTargets
</commit_message>
<xml_diff>
--- a/data/ClueLayout306.xlsx
+++ b/data/ClueLayout306.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20382"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/170d6889d8d02b02/Documents_1D/Education/_Mines/CSCI306/Clue Assignments/CL16 Lets Play/CL16/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Workspace Eclipse\ClueProject\ClueProject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1142" documentId="8_{9B645E34-7536-42D9-BF6C-9EF036B3BE1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{60DE1705-7892-46FF-BD79-AE9CF34BD2EA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2798C1BB-EC5F-4CFC-9F9E-B8C5104B1972}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31140" yWindow="600" windowWidth="17610" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3183,7 +3183,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+      <selection activeCell="AP17" sqref="AP17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>